<commit_message>
Creating ROI calculation function that generates interactive table with ROIs, also small tweaks in the files modifying variable names
</commit_message>
<xml_diff>
--- a/adstocked_media/media_data.xlsx
+++ b/adstocked_media/media_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abeurope-my.sharepoint.com/personal/mattias_mutso_externi_cz/Documents/Documents/AsahiUK_MMM/adstocked_media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{B9ACED8E-5CC5-4528-9E70-B1C800AA62A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0035BA92-B659-41E9-9FFD-0EA482259FA3}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{B9ACED8E-5CC5-4528-9E70-B1C800AA62A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91263D36-7111-456E-98A3-29884D6B8AF2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{08679BA8-D4A7-4C84-AD3C-48D9F272419A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
   <si>
     <t>Date</t>
   </si>
@@ -78,12 +78,6 @@
   </si>
   <si>
     <t>m_vod_peroni_sp</t>
-  </si>
-  <si>
-    <t>m_vod_peroni0_im</t>
-  </si>
-  <si>
-    <t>m_vod_peroni0_sp</t>
   </si>
   <si>
     <t>m_vod_asahi_im</t>
@@ -508,6 +502,18 @@
   <si>
     <t>m_tv_asahi_total_tvr</t>
   </si>
+  <si>
+    <t>m_tv_peroni0_total_sp</t>
+  </si>
+  <si>
+    <t>m_tv_peroni0_total_tvr</t>
+  </si>
+  <si>
+    <t>m_vod_peroni0_peroni0_im</t>
+  </si>
+  <si>
+    <t>m_vod_peroni0_peroni0_sp</t>
+  </si>
 </sst>
 </file>
 
@@ -881,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDA9B9A-9634-4913-9070-7E7AEF315551}">
   <dimension ref="A1:FK157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ER1" workbookViewId="0">
-      <selection activeCell="FA1" sqref="FA1"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BC1" sqref="BC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -895,76 +901,76 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>65</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>66</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>67</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>68</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>70</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>71</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>72</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>73</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>74</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>75</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>76</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>77</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>78</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>79</v>
-      </c>
-      <c r="X1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>81</v>
       </c>
       <c r="Z1" t="s">
         <v>1</v>
@@ -991,52 +997,52 @@
         <v>8</v>
       </c>
       <c r="AH1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>82</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>83</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>84</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>86</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>87</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>89</v>
       </c>
       <c r="AP1" t="s">
         <v>9</v>
       </c>
       <c r="AQ1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AT1" t="s">
         <v>90</v>
       </c>
-      <c r="AR1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>91</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>92</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>93</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>95</v>
       </c>
       <c r="AX1" t="s">
         <v>10</v>
@@ -1051,322 +1057,322 @@
         <v>13</v>
       </c>
       <c r="BB1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BD1" t="s">
         <v>14</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>15</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BJ1" t="s">
         <v>16</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BK1" t="s">
         <v>17</v>
       </c>
-      <c r="BF1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BH1" t="s">
+      <c r="BL1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>25</v>
+      </c>
+      <c r="BT1" t="s">
         <v>98</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BU1" t="s">
         <v>99</v>
       </c>
-      <c r="BJ1" t="s">
-        <v>18</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>19</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>20</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>21</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>22</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>23</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>24</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>25</v>
-      </c>
-      <c r="BR1" t="s">
+      <c r="BV1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CI1" t="s">
         <v>26</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CJ1" t="s">
         <v>27</v>
       </c>
-      <c r="BT1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>106</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>107</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>108</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>109</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>110</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>111</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>112</v>
-      </c>
-      <c r="CG1" t="s">
+      <c r="CK1" t="s">
         <v>113</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CL1" t="s">
         <v>114</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CM1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CO1" t="s">
         <v>28</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CP1" t="s">
         <v>29</v>
       </c>
-      <c r="CK1" t="s">
-        <v>115</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>116</v>
-      </c>
-      <c r="CM1" t="s">
+      <c r="CQ1" t="s">
+        <v>30</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>31</v>
+      </c>
+      <c r="CS1" t="s">
         <v>117</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CT1" t="s">
         <v>118</v>
       </c>
-      <c r="CO1" t="s">
-        <v>30</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CQ1" t="s">
+      <c r="CU1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CY1" t="s">
         <v>32</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CZ1" t="s">
         <v>33</v>
       </c>
-      <c r="CS1" t="s">
-        <v>119</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>120</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>121</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>122</v>
-      </c>
-      <c r="CW1" t="s">
+      <c r="DA1" t="s">
+        <v>34</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>35</v>
+      </c>
+      <c r="DC1" t="s">
         <v>123</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DD1" t="s">
         <v>124</v>
       </c>
-      <c r="CY1" t="s">
-        <v>34</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="DA1" t="s">
+      <c r="DE1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DG1" t="s">
         <v>36</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DH1" t="s">
         <v>37</v>
       </c>
-      <c r="DC1" t="s">
-        <v>125</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>126</v>
-      </c>
-      <c r="DE1" t="s">
+      <c r="DI1" t="s">
+        <v>38</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>39</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>40</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>41</v>
+      </c>
+      <c r="DM1" t="s">
         <v>127</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DN1" t="s">
         <v>128</v>
       </c>
-      <c r="DG1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>39</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>40</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>41</v>
-      </c>
-      <c r="DK1" t="s">
+      <c r="DO1" t="s">
+        <v>129</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>130</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>131</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>135</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>136</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>137</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>138</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>139</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>140</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>141</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>142</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>143</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>144</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>145</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>146</v>
+      </c>
+      <c r="EG1" t="s">
         <v>42</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="EH1" t="s">
         <v>43</v>
       </c>
-      <c r="DM1" t="s">
-        <v>129</v>
-      </c>
-      <c r="DN1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DO1" t="s">
-        <v>131</v>
-      </c>
-      <c r="DP1" t="s">
-        <v>132</v>
-      </c>
-      <c r="DQ1" t="s">
-        <v>133</v>
-      </c>
-      <c r="DR1" t="s">
-        <v>134</v>
-      </c>
-      <c r="DS1" t="s">
-        <v>135</v>
-      </c>
-      <c r="DT1" t="s">
-        <v>136</v>
-      </c>
-      <c r="DU1" t="s">
-        <v>137</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>138</v>
-      </c>
-      <c r="DW1" t="s">
-        <v>139</v>
-      </c>
-      <c r="DX1" t="s">
-        <v>140</v>
-      </c>
-      <c r="DY1" t="s">
-        <v>141</v>
-      </c>
-      <c r="DZ1" t="s">
-        <v>142</v>
-      </c>
-      <c r="EA1" t="s">
-        <v>143</v>
-      </c>
-      <c r="EB1" t="s">
-        <v>144</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>145</v>
-      </c>
-      <c r="ED1" t="s">
-        <v>146</v>
-      </c>
-      <c r="EE1" t="s">
+      <c r="EI1" t="s">
         <v>147</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EJ1" t="s">
         <v>148</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EK1" t="s">
+        <v>149</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>150</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>151</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>152</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>153</v>
+      </c>
+      <c r="EP1" t="s">
         <v>44</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EQ1" t="s">
+        <v>89</v>
+      </c>
+      <c r="ER1" t="s">
         <v>45</v>
       </c>
-      <c r="EI1" t="s">
-        <v>149</v>
-      </c>
-      <c r="EJ1" t="s">
-        <v>150</v>
-      </c>
-      <c r="EK1" t="s">
-        <v>151</v>
-      </c>
-      <c r="EL1" t="s">
-        <v>152</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>153</v>
-      </c>
-      <c r="EN1" t="s">
+      <c r="ES1" t="s">
         <v>154</v>
       </c>
-      <c r="EO1" t="s">
-        <v>155</v>
-      </c>
-      <c r="EP1" t="s">
+      <c r="ET1" t="s">
         <v>46</v>
       </c>
-      <c r="EQ1" t="s">
-        <v>91</v>
-      </c>
-      <c r="ER1" t="s">
+      <c r="EU1" t="s">
         <v>47</v>
       </c>
-      <c r="ES1" t="s">
-        <v>156</v>
-      </c>
-      <c r="ET1" t="s">
+      <c r="EV1" t="s">
         <v>48</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EW1" t="s">
         <v>49</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EX1" t="s">
         <v>50</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EY1" t="s">
         <v>51</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="EZ1" t="s">
         <v>52</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="FA1" t="s">
         <v>53</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FB1" t="s">
         <v>54</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FC1" t="s">
         <v>55</v>
-      </c>
-      <c r="FB1" t="s">
-        <v>56</v>
-      </c>
-      <c r="FC1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:167" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Created new tails function and modified decomp and ROI calculation functions because of tails.
</commit_message>
<xml_diff>
--- a/adstocked_media/media_data.xlsx
+++ b/adstocked_media/media_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abeurope-my.sharepoint.com/personal/mattias_mutso_externi_cz/Documents/Documents/AsahiUK_MMM/adstocked_media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{B9ACED8E-5CC5-4528-9E70-B1C800AA62A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91263D36-7111-456E-98A3-29884D6B8AF2}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{B9ACED8E-5CC5-4528-9E70-B1C800AA62A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79859299-B141-4198-8BE9-2002332DD078}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{08679BA8-D4A7-4C84-AD3C-48D9F272419A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{08679BA8-D4A7-4C84-AD3C-48D9F272419A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>m_influencers_asd_im</t>
-  </si>
-  <si>
-    <t>m_influencers_asd_sp</t>
   </si>
   <si>
     <t>m_influencers_peroni0_im</t>
@@ -264,18 +258,6 @@
   </si>
   <si>
     <t>m_social_peroni0_total_sp</t>
-  </si>
-  <si>
-    <t>m_fb_asd_im</t>
-  </si>
-  <si>
-    <t>m_fb_asd_sp</t>
-  </si>
-  <si>
-    <t>m_ig_asd_im</t>
-  </si>
-  <si>
-    <t>m_ig_asd_sp</t>
   </si>
   <si>
     <t>m_tv_capri_total_sp</t>
@@ -513,6 +495,24 @@
   </si>
   <si>
     <t>m_vod_peroni0_peroni0_sp</t>
+  </si>
+  <si>
+    <t>m_fb_asahi_im</t>
+  </si>
+  <si>
+    <t>m_fb_asahi_sp</t>
+  </si>
+  <si>
+    <t>m_ig_asahi_im</t>
+  </si>
+  <si>
+    <t>m_ig_asahi_sp</t>
+  </si>
+  <si>
+    <t>m_influencers_asahi_im</t>
+  </si>
+  <si>
+    <t>m_influencers_asahi_sp</t>
   </si>
 </sst>
 </file>
@@ -888,494 +888,494 @@
   <dimension ref="A1:FK157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BC1" sqref="BC1"/>
+      <selection activeCell="AW14" sqref="AW14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>67</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>68</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>69</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>71</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>72</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>73</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W1" t="s">
+        <v>154</v>
+      </c>
+      <c r="X1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH1" t="s">
         <v>74</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AI1" t="s">
         <v>75</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AJ1" t="s">
         <v>76</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AK1" t="s">
         <v>77</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AL1" t="s">
         <v>78</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AM1" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AN1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP1" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AQ1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX1" t="s">
         <v>8</v>
       </c>
-      <c r="AH1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK1" t="s">
+      <c r="AY1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>152</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>15</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>16</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>17</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>106</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>24</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>25</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>26</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>27</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>28</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>30</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>31</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>32</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>33</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>117</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>118</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>119</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>120</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>34</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>35</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>37</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>38</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>39</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>125</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>126</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>128</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>129</v>
+      </c>
+      <c r="DV1" t="s">
+        <v>130</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>131</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>134</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>135</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>136</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>137</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>138</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>139</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>140</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>40</v>
+      </c>
+      <c r="EH1" t="s">
+        <v>41</v>
+      </c>
+      <c r="EI1" t="s">
+        <v>141</v>
+      </c>
+      <c r="EJ1" t="s">
+        <v>142</v>
+      </c>
+      <c r="EK1" t="s">
+        <v>143</v>
+      </c>
+      <c r="EL1" t="s">
+        <v>144</v>
+      </c>
+      <c r="EM1" t="s">
+        <v>145</v>
+      </c>
+      <c r="EN1" t="s">
+        <v>146</v>
+      </c>
+      <c r="EO1" t="s">
+        <v>147</v>
+      </c>
+      <c r="EP1" t="s">
+        <v>42</v>
+      </c>
+      <c r="EQ1" t="s">
         <v>83</v>
       </c>
-      <c r="AL1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>12</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>157</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>158</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>96</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>17</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>18</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>19</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>20</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>21</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>22</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>23</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>24</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>25</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>98</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>104</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>105</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>106</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>107</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>108</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>109</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>110</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>111</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>112</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>26</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>27</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>113</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>114</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>115</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>116</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>28</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>29</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>30</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>117</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>118</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>119</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>120</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>121</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>122</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>32</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>33</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>34</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>35</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>123</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>124</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>125</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>126</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>37</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>39</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>40</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>41</v>
-      </c>
-      <c r="DM1" t="s">
-        <v>127</v>
-      </c>
-      <c r="DN1" t="s">
-        <v>128</v>
-      </c>
-      <c r="DO1" t="s">
-        <v>129</v>
-      </c>
-      <c r="DP1" t="s">
-        <v>130</v>
-      </c>
-      <c r="DQ1" t="s">
-        <v>131</v>
-      </c>
-      <c r="DR1" t="s">
-        <v>132</v>
-      </c>
-      <c r="DS1" t="s">
-        <v>133</v>
-      </c>
-      <c r="DT1" t="s">
-        <v>134</v>
-      </c>
-      <c r="DU1" t="s">
-        <v>135</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>136</v>
-      </c>
-      <c r="DW1" t="s">
-        <v>137</v>
-      </c>
-      <c r="DX1" t="s">
-        <v>138</v>
-      </c>
-      <c r="DY1" t="s">
-        <v>139</v>
-      </c>
-      <c r="DZ1" t="s">
-        <v>140</v>
-      </c>
-      <c r="EA1" t="s">
-        <v>141</v>
-      </c>
-      <c r="EB1" t="s">
-        <v>142</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>143</v>
-      </c>
-      <c r="ED1" t="s">
-        <v>144</v>
-      </c>
-      <c r="EE1" t="s">
-        <v>145</v>
-      </c>
-      <c r="EF1" t="s">
-        <v>146</v>
-      </c>
-      <c r="EG1" t="s">
-        <v>42</v>
-      </c>
-      <c r="EH1" t="s">
+      <c r="ER1" t="s">
         <v>43</v>
       </c>
-      <c r="EI1" t="s">
-        <v>147</v>
-      </c>
-      <c r="EJ1" t="s">
+      <c r="ES1" t="s">
         <v>148</v>
       </c>
-      <c r="EK1" t="s">
-        <v>149</v>
-      </c>
-      <c r="EL1" t="s">
-        <v>150</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>151</v>
-      </c>
-      <c r="EN1" t="s">
-        <v>152</v>
-      </c>
-      <c r="EO1" t="s">
-        <v>153</v>
-      </c>
-      <c r="EP1" t="s">
+      <c r="ET1" t="s">
         <v>44</v>
       </c>
-      <c r="EQ1" t="s">
-        <v>89</v>
-      </c>
-      <c r="ER1" t="s">
+      <c r="EU1" t="s">
         <v>45</v>
       </c>
-      <c r="ES1" t="s">
-        <v>154</v>
-      </c>
-      <c r="ET1" t="s">
+      <c r="EV1" t="s">
         <v>46</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EW1" t="s">
         <v>47</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EX1" t="s">
         <v>48</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EY1" t="s">
         <v>49</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="EZ1" t="s">
         <v>50</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="FA1" t="s">
         <v>51</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FB1" t="s">
         <v>52</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FC1" t="s">
         <v>53</v>
       </c>
-      <c r="FB1" t="s">
-        <v>54</v>
-      </c>
-      <c r="FC1" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="2" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44199</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44206</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44213</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44220</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:167" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44227</v>
       </c>
@@ -3775,7 +3775,7 @@
       <c r="FJ6" s="4"/>
       <c r="FK6" s="4"/>
     </row>
-    <row r="7" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:167" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44234</v>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="FJ7" s="4"/>
       <c r="FK7" s="4"/>
     </row>
-    <row r="8" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44241</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44248</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44255</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44262</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44269</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44276</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44283</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44290</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:167" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44297</v>
       </c>
@@ -8570,7 +8570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44304</v>
       </c>
@@ -9049,7 +9049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44311</v>
       </c>
@@ -9528,7 +9528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44318</v>
       </c>
@@ -10007,7 +10007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44325</v>
       </c>
@@ -10486,7 +10486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44332</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44339</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44346</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44353</v>
       </c>
@@ -12402,7 +12402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44360</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>44367</v>
       </c>
@@ -13360,7 +13360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>44374</v>
       </c>
@@ -13839,7 +13839,7 @@
         <v>8582362</v>
       </c>
     </row>
-    <row r="28" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44381</v>
       </c>
@@ -14318,7 +14318,7 @@
         <v>10771066</v>
       </c>
     </row>
-    <row r="29" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44388</v>
       </c>
@@ -14797,7 +14797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>44395</v>
       </c>
@@ -15276,7 +15276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44402</v>
       </c>
@@ -15755,7 +15755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44409</v>
       </c>
@@ -16234,7 +16234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44416</v>
       </c>
@@ -16713,7 +16713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>44423</v>
       </c>
@@ -17192,7 +17192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44430</v>
       </c>
@@ -17671,7 +17671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>44437</v>
       </c>
@@ -18150,7 +18150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>44444</v>
       </c>
@@ -18629,7 +18629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>44451</v>
       </c>
@@ -19108,7 +19108,7 @@
         <v>4134244</v>
       </c>
     </row>
-    <row r="39" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>44458</v>
       </c>
@@ -19587,7 +19587,7 @@
         <v>4134244</v>
       </c>
     </row>
-    <row r="40" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>44465</v>
       </c>
@@ -20066,7 +20066,7 @@
         <v>8503005</v>
       </c>
     </row>
-    <row r="41" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>44472</v>
       </c>
@@ -20545,7 +20545,7 @@
         <v>4368760</v>
       </c>
     </row>
-    <row r="42" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>44479</v>
       </c>
@@ -21024,7 +21024,7 @@
         <v>3532690</v>
       </c>
     </row>
-    <row r="43" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>44486</v>
       </c>
@@ -21503,7 +21503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44493</v>
       </c>
@@ -21982,7 +21982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44500</v>
       </c>
@@ -22461,7 +22461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44507</v>
       </c>
@@ -22940,7 +22940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>44514</v>
       </c>
@@ -23419,7 +23419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>44521</v>
       </c>
@@ -23898,7 +23898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>44528</v>
       </c>
@@ -24377,7 +24377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>44535</v>
       </c>
@@ -24856,7 +24856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>44542</v>
       </c>
@@ -25335,7 +25335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>44549</v>
       </c>
@@ -25814,7 +25814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>44556</v>
       </c>
@@ -26293,7 +26293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>44563</v>
       </c>
@@ -26772,7 +26772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>44570</v>
       </c>
@@ -27251,7 +27251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>44577</v>
       </c>
@@ -27730,7 +27730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>44584</v>
       </c>
@@ -28209,7 +28209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>44591</v>
       </c>
@@ -28688,7 +28688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>44598</v>
       </c>
@@ -29167,7 +29167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>44605</v>
       </c>
@@ -29646,7 +29646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>44612</v>
       </c>
@@ -30125,7 +30125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>44619</v>
       </c>
@@ -30604,7 +30604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>44626</v>
       </c>
@@ -31083,7 +31083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>44633</v>
       </c>
@@ -31562,7 +31562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>44640</v>
       </c>
@@ -32041,7 +32041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>44647</v>
       </c>
@@ -32520,7 +32520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>44654</v>
       </c>
@@ -32999,7 +32999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>44661</v>
       </c>
@@ -33478,7 +33478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>44668</v>
       </c>
@@ -33957,7 +33957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>44675</v>
       </c>
@@ -34436,7 +34436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>44682</v>
       </c>
@@ -34915,7 +34915,7 @@
         <v>75503325</v>
       </c>
     </row>
-    <row r="72" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>44689</v>
       </c>
@@ -35394,7 +35394,7 @@
         <v>74513696</v>
       </c>
     </row>
-    <row r="73" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>44696</v>
       </c>
@@ -35873,7 +35873,7 @@
         <v>32218482</v>
       </c>
     </row>
-    <row r="74" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>44703</v>
       </c>
@@ -36352,7 +36352,7 @@
         <v>34833419</v>
       </c>
     </row>
-    <row r="75" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>44710</v>
       </c>
@@ -36831,7 +36831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>44717</v>
       </c>
@@ -37310,7 +37310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>44724</v>
       </c>
@@ -37789,7 +37789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>44731</v>
       </c>
@@ -38268,7 +38268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>44738</v>
       </c>
@@ -38747,7 +38747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>44745</v>
       </c>
@@ -39226,7 +39226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>44752</v>
       </c>
@@ -39705,7 +39705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>44759</v>
       </c>
@@ -40184,7 +40184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>44766</v>
       </c>
@@ -40663,7 +40663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>44773</v>
       </c>
@@ -41142,7 +41142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>44780</v>
       </c>
@@ -41621,7 +41621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>44787</v>
       </c>
@@ -42100,7 +42100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>44794</v>
       </c>
@@ -42579,7 +42579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>44801</v>
       </c>
@@ -43058,7 +43058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>44808</v>
       </c>
@@ -43537,7 +43537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>44815</v>
       </c>
@@ -44016,7 +44016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>44822</v>
       </c>
@@ -44495,7 +44495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>44829</v>
       </c>
@@ -44974,7 +44974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>44836</v>
       </c>
@@ -45453,7 +45453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>44843</v>
       </c>
@@ -45932,7 +45932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>44850</v>
       </c>
@@ -46411,7 +46411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>44857</v>
       </c>
@@ -46890,7 +46890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>44864</v>
       </c>
@@ -47369,7 +47369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>44871</v>
       </c>
@@ -47848,7 +47848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>44878</v>
       </c>
@@ -48327,7 +48327,7 @@
         <v>172805568</v>
       </c>
     </row>
-    <row r="100" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>44885</v>
       </c>
@@ -48806,7 +48806,7 @@
         <v>173064019</v>
       </c>
     </row>
-    <row r="101" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>44892</v>
       </c>
@@ -49285,7 +49285,7 @@
         <v>44156528</v>
       </c>
     </row>
-    <row r="102" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>44899</v>
       </c>
@@ -49764,7 +49764,7 @@
         <v>44156528</v>
       </c>
     </row>
-    <row r="103" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>44906</v>
       </c>
@@ -50243,7 +50243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>44913</v>
       </c>
@@ -50722,7 +50722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>44920</v>
       </c>
@@ -51201,7 +51201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>44927</v>
       </c>
@@ -51680,7 +51680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>44934</v>
       </c>
@@ -52159,7 +52159,7 @@
         <v>20872432</v>
       </c>
     </row>
-    <row r="108" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>44941</v>
       </c>
@@ -52638,7 +52638,7 @@
         <v>21011262</v>
       </c>
     </row>
-    <row r="109" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>44948</v>
       </c>
@@ -53117,7 +53117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>44955</v>
       </c>
@@ -53596,7 +53596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>44962</v>
       </c>
@@ -54075,7 +54075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>44969</v>
       </c>
@@ -54554,7 +54554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>44976</v>
       </c>
@@ -55033,7 +55033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>44983</v>
       </c>
@@ -55512,7 +55512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>44990</v>
       </c>
@@ -55991,7 +55991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>44997</v>
       </c>
@@ -56470,7 +56470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>45004</v>
       </c>
@@ -56949,7 +56949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>45011</v>
       </c>
@@ -57428,7 +57428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>45018</v>
       </c>
@@ -57907,7 +57907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>45025</v>
       </c>
@@ -58386,7 +58386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>45032</v>
       </c>
@@ -58865,7 +58865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>45039</v>
       </c>
@@ -59344,7 +59344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>45046</v>
       </c>
@@ -59823,7 +59823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>45053</v>
       </c>
@@ -60302,7 +60302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>45060</v>
       </c>
@@ -60781,7 +60781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>45067</v>
       </c>
@@ -61260,7 +61260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>45074</v>
       </c>
@@ -61739,7 +61739,7 @@
         <v>154444995</v>
       </c>
     </row>
-    <row r="128" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>45081</v>
       </c>
@@ -62218,7 +62218,7 @@
         <v>154410284</v>
       </c>
     </row>
-    <row r="129" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>45088</v>
       </c>
@@ -62697,7 +62697,7 @@
         <v>25823727</v>
       </c>
     </row>
-    <row r="130" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>45095</v>
       </c>
@@ -63176,7 +63176,7 @@
         <v>25823727</v>
       </c>
     </row>
-    <row r="131" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>45102</v>
       </c>
@@ -63655,7 +63655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>45109</v>
       </c>
@@ -64134,7 +64134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>45116</v>
       </c>
@@ -64613,7 +64613,7 @@
         <v>21747975</v>
       </c>
     </row>
-    <row r="134" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>45123</v>
       </c>
@@ -65092,7 +65092,7 @@
         <v>21747975</v>
       </c>
     </row>
-    <row r="135" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>45130</v>
       </c>
@@ -65571,7 +65571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>45137</v>
       </c>
@@ -66050,7 +66050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>45144</v>
       </c>
@@ -66529,7 +66529,7 @@
         <v>24165755</v>
       </c>
     </row>
-    <row r="138" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>45151</v>
       </c>
@@ -67008,7 +67008,7 @@
         <v>24165755</v>
       </c>
     </row>
-    <row r="139" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>45158</v>
       </c>
@@ -67487,7 +67487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>45165</v>
       </c>
@@ -67966,7 +67966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>45172</v>
       </c>
@@ -68445,7 +68445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>45179</v>
       </c>
@@ -68924,7 +68924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>45186</v>
       </c>
@@ -69403,7 +69403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>45193</v>
       </c>
@@ -69882,7 +69882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>45200</v>
       </c>
@@ -70361,7 +70361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>45207</v>
       </c>
@@ -70840,7 +70840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>45214</v>
       </c>
@@ -71319,7 +71319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>45221</v>
       </c>
@@ -71798,7 +71798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>45228</v>
       </c>
@@ -72277,7 +72277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>45235</v>
       </c>
@@ -72756,7 +72756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>45242</v>
       </c>
@@ -73235,7 +73235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>45249</v>
       </c>
@@ -73714,7 +73714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>45256</v>
       </c>
@@ -74193,7 +74193,7 @@
         <v>51947030</v>
       </c>
     </row>
-    <row r="154" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>45263</v>
       </c>
@@ -74672,7 +74672,7 @@
         <v>51947030</v>
       </c>
     </row>
-    <row r="155" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>45270</v>
       </c>
@@ -75151,7 +75151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>45277</v>
       </c>
@@ -75630,7 +75630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>45284</v>
       </c>

</xml_diff>